<commit_message>
uploaded most of the available vkg in ontop-examples
</commit_message>
<xml_diff>
--- a/vkg_resources_xhh.xlsx
+++ b/vkg_resources_xhh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\vkg_resource_collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7F4B67-3CD5-42C6-A755-C1E969BCF949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA03142-0269-41B9-AEEE-196353EC2F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13536" yWindow="5820" windowWidth="14484" windowHeight="8844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>VKG name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>uobm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Related URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://github.com/ontop/ontop-examples/tree/master/aaai-2016-ontoprox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ontology</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -67,6 +59,66 @@
   </si>
   <si>
     <t>MySQL</t>
+  </si>
+  <si>
+    <t>bsbm</t>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/dke-2022-mapping-patterns/scenarios</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/caise-2021-patterns/scenarios/npd</t>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/caise-2021-patterns/scenarios/cordis</t>
+  </si>
+  <si>
+    <t>cordis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suedtirol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/dke-2022-mapping-patterns/scenarios/suedtirol-open-data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canonical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/eswc-2018-canonical-iri</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dblp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/ontop/ontop-examples/tree/master/swj-2017-vig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -411,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -433,45 +485,160 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -482,9 +649,12 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A42A59F8-5ED6-43EA-92A2-EA5E5892CA53}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5127476F-F75E-42DE-A780-D38A49B43D20}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{9E7C72C4-41F1-4D1A-9077-61A68E368B4C}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{C6A5E01B-A4FF-415B-8B0F-B16671602D21}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{EB883D40-8DAC-48FF-A006-F396749403E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>